<commit_message>
fix: update export pendapatan in laporan pendapatan
</commit_message>
<xml_diff>
--- a/public/export_template/template_pendapatan.xlsx
+++ b/public/export_template/template_pendapatan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753D6A30-4E98-4AA5-ACF2-D41EBA8DF026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0653A685-A81B-4334-8697-901646327CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{80DC0547-5610-42A6-8E16-3EFBB5419B10}"/>
   </bookViews>
@@ -151,14 +151,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -166,23 +163,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F79EA71-1037-4063-AE2C-9F084DE21A77}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,117 +530,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="11"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
fix: update Pendapatan export template and adjust column mappings
</commit_message>
<xml_diff>
--- a/public/export_template/template_pendapatan.xlsx
+++ b/public/export_template/template_pendapatan.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0653A685-A81B-4334-8697-901646327CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714EE359-BDC8-44B0-A440-6B54F44DE927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{80DC0547-5610-42A6-8E16-3EFBB5419B10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{80DC0547-5610-42A6-8E16-3EFBB5419B10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>BDR BALL</t>
   </si>
@@ -84,6 +82,9 @@
   </si>
   <si>
     <t>Laba Bersih</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -151,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,20 +161,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -512,135 +525,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F79EA71-1037-4063-AE2C-9F084DE21A77}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="11"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="8"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="C18" s="13"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
+  <mergeCells count="9">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: laporan pendapatan export excel
</commit_message>
<xml_diff>
--- a/public/export_template/template_pendapatan.xlsx
+++ b/public/export_template/template_pendapatan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714EE359-BDC8-44B0-A440-6B54F44DE927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7AFDC3-C991-4073-9A5F-A04EEAFA142F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{80DC0547-5610-42A6-8E16-3EFBB5419B10}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>BDR BALL</t>
   </si>
@@ -61,27 +61,6 @@
   </si>
   <si>
     <t>Jumlah Penjualan</t>
-  </si>
-  <si>
-    <t>Total Penjualan</t>
-  </si>
-  <si>
-    <t>Total Diskon Produk</t>
-  </si>
-  <si>
-    <t>Total Diskon Nota</t>
-  </si>
-  <si>
-    <t>Total Pengeluaran</t>
-  </si>
-  <si>
-    <t>Total Transfer</t>
-  </si>
-  <si>
-    <t>Modal Usaha</t>
-  </si>
-  <si>
-    <t>Laba Bersih</t>
   </si>
   <si>
     <t>No</t>
@@ -180,17 +159,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +505,7 @@
   <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,34 +520,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>2</v>
@@ -616,64 +593,45 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C20" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
+  <mergeCells count="2">
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>